<commit_message>
Commited changes for the correct password
</commit_message>
<xml_diff>
--- a/UploadData/Sigin.xlsx
+++ b/UploadData/Sigin.xlsx
@@ -41,7 +41,7 @@
     <t>kinjal</t>
   </si>
   <si>
-    <t>maury</t>
+    <t>maurya</t>
   </si>
 </sst>
 </file>
@@ -362,7 +362,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>